<commit_message>
add negative validation scenarios in Authenticate API
</commit_message>
<xml_diff>
--- a/test-cases/TestCases.xlsx
+++ b/test-cases/TestCases.xlsx
@@ -239,8 +239,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -254,6 +254,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -268,6 +297,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -275,18 +342,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -298,9 +366,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,89 +396,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -412,24 +412,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -442,7 +520,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,7 +538,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,19 +562,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,109 +586,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,6 +621,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -632,6 +641,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,15 +671,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -671,6 +682,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -692,38 +718,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -732,139 +732,139 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1205,10 +1205,10 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.8571428571429" defaultRowHeight="15"/>
@@ -1361,7 +1361,7 @@
         <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>15</v>
@@ -1390,7 +1390,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>15</v>
@@ -1419,7 +1419,7 @@
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>15</v>
@@ -1506,7 +1506,7 @@
         <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>14</v>
@@ -1533,7 +1533,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>15</v>
@@ -1618,7 +1618,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>14</v>
@@ -1645,7 +1645,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>15</v>

</xml_diff>